<commit_message>
Daily attendance processing - 2026-02-08 04:51:33 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -484,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="28" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="S22" s="5" t="inlineStr">
         <is>
-          <t>22.1%</t>
+          <t>22.5%</t>
         </is>
       </c>
     </row>
@@ -5733,7 +5733,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G111" s="2" t="inlineStr"/>
+      <c r="G111" s="2" t="inlineStr">
+        <is>
+          <t>Wafaa.ebida@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H111" s="2" t="inlineStr">
         <is>
           <t>24/154</t>
@@ -6679,7 +6683,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G133" s="2" t="inlineStr"/>
+      <c r="G133" s="2" t="inlineStr">
+        <is>
+          <t>Wafaa.ebida@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H133" s="2" t="inlineStr">
         <is>
           <t>60/224</t>
@@ -7625,7 +7633,11 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G155" s="2" t="inlineStr"/>
+      <c r="G155" s="2" t="inlineStr">
+        <is>
+          <t>Wafaa.ebida@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H155" s="2" t="inlineStr">
         <is>
           <t>34/224</t>
@@ -8571,10 +8583,14 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G177" s="2" t="inlineStr"/>
+      <c r="G177" s="2" t="inlineStr">
+        <is>
+          <t>Wafaa.ebida@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H177" s="2" t="inlineStr">
         <is>
-          <t>17/226</t>
+          <t>32/226</t>
         </is>
       </c>
       <c r="I177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 07:06:17 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -484,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="28" customWidth="1" min="7" max="7"/>
+    <col width="32" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
@@ -950,7 +950,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>75.0%</t>
+          <t>75.6%</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>39.4%</t>
+          <t>40.0%</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>41.4%</t>
+          <t>42.6%</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="S18" s="5" t="inlineStr">
         <is>
-          <t>34.6%</t>
+          <t>35.2%</t>
         </is>
       </c>
     </row>
@@ -1728,10 +1728,14 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G21" s="2" t="inlineStr"/>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>neveen.nashaat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>52/216</t>
+          <t>80/216</t>
         </is>
       </c>
       <c r="I21" s="2" t="inlineStr">
@@ -1834,22 +1838,22 @@
         <v>22</v>
       </c>
       <c r="O22" s="5" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P22" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q22" s="5" t="n">
         <v>0</v>
       </c>
       <c r="R22" s="5" t="inlineStr">
         <is>
-          <t>72.7%</t>
+          <t>77.3%</t>
         </is>
       </c>
       <c r="S22" s="5" t="inlineStr">
         <is>
-          <t>22.5%</t>
+          <t>21.2%</t>
         </is>
       </c>
     </row>
@@ -2809,7 +2813,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G43" s="2" t="inlineStr"/>
+      <c r="G43" s="2" t="inlineStr">
+        <is>
+          <t>neveen.nashaat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
           <t>41/217</t>
@@ -3669,10 +3677,14 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G63" s="2" t="inlineStr"/>
+      <c r="G63" s="2" t="inlineStr">
+        <is>
+          <t>neveen.nashaat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H63" s="2" t="inlineStr">
         <is>
-          <t>74/220</t>
+          <t>97/220</t>
         </is>
       </c>
       <c r="I63" s="2" t="inlineStr">
@@ -3712,7 +3724,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G64" s="2" t="inlineStr"/>
+      <c r="G64" s="2" t="inlineStr">
+        <is>
+          <t>neveen.nashaat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
           <t>20/220</t>
@@ -3755,10 +3771,14 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G65" s="2" t="inlineStr"/>
+      <c r="G65" s="2" t="inlineStr">
+        <is>
+          <t>neveen.nashaat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H65" s="2" t="inlineStr">
         <is>
-          <t>104/220</t>
+          <t>123/220</t>
         </is>
       </c>
       <c r="I65" s="2" t="inlineStr">
@@ -4615,7 +4635,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G85" s="2" t="inlineStr"/>
+      <c r="G85" s="2" t="inlineStr">
+        <is>
+          <t>neveen.nashaat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H85" s="2" t="inlineStr">
         <is>
           <t>78/225</t>
@@ -4658,10 +4682,14 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G86" s="2" t="inlineStr"/>
+      <c r="G86" s="2" t="inlineStr">
+        <is>
+          <t>neveen.nashaat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H86" s="2" t="inlineStr">
         <is>
-          <t>32/225</t>
+          <t>55/225</t>
         </is>
       </c>
       <c r="I86" s="2" t="inlineStr">
@@ -4701,7 +4729,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G87" s="2" t="inlineStr"/>
+      <c r="G87" s="2" t="inlineStr">
+        <is>
+          <t>neveen.nashaat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H87" s="2" t="inlineStr">
         <is>
           <t>64/225</t>
@@ -7289,7 +7321,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G147" s="2" t="inlineStr"/>
+      <c r="G147" s="2" t="inlineStr">
+        <is>
+          <t>nourhan.mostafa@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H147" s="2" t="inlineStr">
         <is>
           <t>21/224</t>
@@ -8209,45 +8245,49 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B169" s="4" t="inlineStr">
+      <c r="A169" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B169" s="2" t="inlineStr">
         <is>
           <t>B4</t>
         </is>
       </c>
-      <c r="C169" s="4" t="inlineStr">
+      <c r="C169" s="2" t="inlineStr">
         <is>
           <t>PHARMACOLOGY</t>
         </is>
       </c>
-      <c r="D169" s="4" t="inlineStr">
+      <c r="D169" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E169" s="4" t="inlineStr">
+      <c r="E169" s="2" t="inlineStr">
         <is>
           <t>11/12/2025</t>
         </is>
       </c>
-      <c r="F169" s="4" t="inlineStr">
+      <c r="F169" s="2" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G169" s="4" t="inlineStr"/>
-      <c r="H169" s="4" t="inlineStr">
-        <is>
-          <t>0/226</t>
-        </is>
-      </c>
-      <c r="I169" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="G169" s="2" t="inlineStr">
+        <is>
+          <t>nourhan.mostafa@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H169" s="2" t="inlineStr">
+        <is>
+          <t>2/226</t>
+        </is>
+      </c>
+      <c r="I169" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 08:38:07 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -7192,7 +7192,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G144" s="2" t="inlineStr"/>
+      <c r="G144" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H144" s="2" t="inlineStr">
         <is>
           <t>168/224</t>
@@ -8146,7 +8150,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G166" s="2" t="inlineStr"/>
+      <c r="G166" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H166" s="2" t="inlineStr">
         <is>
           <t>118/226</t>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-09 07:11:10 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -7106,7 +7106,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G142" s="2" t="inlineStr"/>
+      <c r="G142" s="2" t="inlineStr">
+        <is>
+          <t>marwa_mustafa@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H142" s="2" t="inlineStr">
         <is>
           <t>140/224</t>
@@ -8064,7 +8068,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G164" s="2" t="inlineStr"/>
+      <c r="G164" s="2" t="inlineStr">
+        <is>
+          <t>marwa_mustafa@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H164" s="2" t="inlineStr">
         <is>
           <t>91/226</t>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-10 11:05:55 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7">
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
@@ -950,7 +950,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>75.6%</t>
+          <t>76.1%</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>38.6%</t>
+          <t>38.5%</t>
         </is>
       </c>
     </row>
@@ -1444,22 +1444,22 @@
         <v>22</v>
       </c>
       <c r="O17" s="5" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q17" s="5" t="n">
         <v>0</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
-          <t>72.7%</t>
+          <t>77.3%</t>
         </is>
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>42.6%</t>
+          <t>41.0%</t>
         </is>
       </c>
     </row>
@@ -3475,45 +3475,49 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B59" s="4" t="inlineStr">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
         <is>
           <t>A3</t>
         </is>
       </c>
-      <c r="C59" s="4" t="inlineStr">
+      <c r="C59" s="2" t="inlineStr">
         <is>
           <t>PHARMACOLOGY</t>
         </is>
       </c>
-      <c r="D59" s="4" t="inlineStr">
+      <c r="D59" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E59" s="4" t="inlineStr">
+      <c r="E59" s="2" t="inlineStr">
         <is>
           <t>09/12/2025</t>
         </is>
       </c>
-      <c r="F59" s="4" t="inlineStr">
+      <c r="F59" s="2" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G59" s="4" t="inlineStr"/>
-      <c r="H59" s="4" t="inlineStr">
-        <is>
-          <t>0/220</t>
-        </is>
-      </c>
-      <c r="I59" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="G59" s="2" t="inlineStr">
+        <is>
+          <t>marian.samir@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H59" s="2" t="inlineStr">
+        <is>
+          <t>34/220</t>
+        </is>
+      </c>
+      <c r="I59" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -4463,7 +4467,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G81" s="2" t="inlineStr"/>
+      <c r="G81" s="2" t="inlineStr">
+        <is>
+          <t>marian.samir@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H81" s="2" t="inlineStr">
         <is>
           <t>26/225</t>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-10 12:00:01 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -484,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="32" customWidth="1" min="7" max="7"/>
+    <col width="34" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -3032,7 +3032,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G48" s="2" t="inlineStr"/>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
           <t>63/220</t>
@@ -3994,7 +3998,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G70" s="2" t="inlineStr"/>
+      <c r="G70" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H70" s="2" t="inlineStr">
         <is>
           <t>60/225</t>
@@ -4956,7 +4964,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G92" s="2" t="inlineStr"/>
+      <c r="G92" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H92" s="2" t="inlineStr">
         <is>
           <t>120/154</t>
@@ -5906,7 +5918,11 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G114" s="2" t="inlineStr"/>
+      <c r="G114" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H114" s="2" t="inlineStr">
         <is>
           <t>162/224</t>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 13:10:43 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -484,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="34" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 14:24:33 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 17:47:30 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 23:36:16 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 04:32:51 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 05:54:18 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 07:59:36 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 08:50:21 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 11:40:36 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 12:05:04 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 15:00:58 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 15:50:02 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 17:49:46 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 18:53:45 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 21:43:38 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-13 22:38:32 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-14 01:58:39 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-14 04:19:09 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-14 05:40:05 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-14 06:17:35 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-14 07:19:13 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-14 08:05:23 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
+          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-14 09:08:09 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -5787,7 +5787,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -8665,7 +8665,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>eman.samir@med.asu.edu.eg, Wafaa.ebida@med.asu.edu.eg</t>
+          <t>Wafaa.ebida@med.asu.edu.eg, eman.samir@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-18 15:24:57 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -1302,7 +1302,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2023/2024</t>
+          <t>2023/2024, 2025/2026</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, Eman_mohamed@med.asu.edu.eg</t>
+          <t>Eman_mohamed@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H22" s="2" t="inlineStr">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="G37" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2023/2024</t>
+          <t>2023/2024, 2025/2026</t>
         </is>
       </c>
       <c r="H37" s="2" t="inlineStr">
@@ -2994,7 +2994,7 @@
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, Eman_mohamed@med.asu.edu.eg</t>
+          <t>Eman_mohamed@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H44" s="2" t="inlineStr">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2026/2027</t>
+          <t>2026/2027, 2025/2026</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="G82" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2026/2027</t>
+          <t>2026/2027, 2025/2026</t>
         </is>
       </c>
       <c r="H82" s="2" t="inlineStr">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="G104" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2026/2027</t>
+          <t>2026/2027, 2025/2026</t>
         </is>
       </c>
       <c r="H104" s="2" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
+          <t>yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6764,7 +6764,7 @@
       </c>
       <c r="G126" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2026/2027</t>
+          <t>2026/2027, 2025/2026</t>
         </is>
       </c>
       <c r="H126" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
+          <t>yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
+          <t>yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
+          <t>yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-18 20:47:20 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>yassmen.ahmed@med.asu.edu.eg, 2025/2026, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>yassmen.ahmed@med.asu.edu.eg, 2025/2026, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>yassmen.ahmed@med.asu.edu.eg, 2025/2026, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>yassmen.ahmed@med.asu.edu.eg, 2025/2026, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-20 02:01:26 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, 2025/2026</t>
+          <t>marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, 2025/2026</t>
+          <t>marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, 2025/2026</t>
+          <t>marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, 2025/2026</t>
+          <t>marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-20 05:48:12 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg</t>
+          <t>youstina.magdy@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, 2025/2026, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg</t>
+          <t>youstina.magdy@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, 2025/2026, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg</t>
+          <t>youstina.magdy@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, 2025/2026, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg</t>
+          <t>youstina.magdy@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, 2025/2026, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-20 19:47:19 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -3734,7 +3734,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2026/2027</t>
+          <t>2026/2027, 2025/2026</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="G82" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2026/2027</t>
+          <t>2026/2027, 2025/2026</t>
         </is>
       </c>
       <c r="H82" s="2" t="inlineStr">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="G104" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2026/2027</t>
+          <t>2026/2027, 2025/2026</t>
         </is>
       </c>
       <c r="H104" s="2" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
+          <t>yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6764,7 +6764,7 @@
       </c>
       <c r="G126" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, 2026/2027</t>
+          <t>2026/2027, 2025/2026</t>
         </is>
       </c>
       <c r="H126" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
+          <t>yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
+          <t>yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg</t>
+          <t>yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-21 13:52:29 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -1876,7 +1876,7 @@
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>Eman_mohamed@med.asu.edu.eg, 2025/2026</t>
+          <t>2025/2026, Eman_mohamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H22" s="2" t="inlineStr">
@@ -2994,7 +2994,7 @@
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>Eman_mohamed@med.asu.edu.eg, 2025/2026</t>
+          <t>2025/2026, Eman_mohamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H44" s="2" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026, yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-21 16:36:47 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -1876,7 +1876,7 @@
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, Eman_mohamed@med.asu.edu.eg</t>
+          <t>Eman_mohamed@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H22" s="2" t="inlineStr">
@@ -2994,7 +2994,7 @@
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>2025/2026, Eman_mohamed@med.asu.edu.eg</t>
+          <t>Eman_mohamed@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H44" s="2" t="inlineStr">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>2026/2027, 2025/2026</t>
+          <t>2025/2026, 2026/2027</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="G82" s="2" t="inlineStr">
         <is>
-          <t>2026/2027, 2025/2026</t>
+          <t>2025/2026, 2026/2027</t>
         </is>
       </c>
       <c r="H82" s="2" t="inlineStr">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="G104" s="2" t="inlineStr">
         <is>
-          <t>2026/2027, 2025/2026</t>
+          <t>2025/2026, 2026/2027</t>
         </is>
       </c>
       <c r="H104" s="2" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026</t>
+          <t>2025/2026, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -6764,7 +6764,7 @@
       </c>
       <c r="G126" s="2" t="inlineStr">
         <is>
-          <t>2026/2027, 2025/2026</t>
+          <t>2025/2026, 2026/2027</t>
         </is>
       </c>
       <c r="H126" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026</t>
+          <t>2025/2026, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026</t>
+          <t>2025/2026, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026</t>
+          <t>2025/2026, youstina.magdy@med.asu.edu.eg, marina_atef@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-21 19:13:50 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026, youstina.magdy@med.asu.edu.eg</t>
+          <t>2025/2026, neveen.nashaat@med.asu.edu.eg, marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026, youstina.magdy@med.asu.edu.eg</t>
+          <t>2025/2026, neveen.nashaat@med.asu.edu.eg, marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026, youstina.magdy@med.asu.edu.eg</t>
+          <t>2025/2026, neveen.nashaat@med.asu.edu.eg, marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, 2025/2026, youstina.magdy@med.asu.edu.eg</t>
+          <t>2025/2026, neveen.nashaat@med.asu.edu.eg, marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-21 23:02:04 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_CVS_session_analysis.xlsx
@@ -6083,7 +6083,7 @@
       </c>
       <c r="G111" s="2" t="inlineStr">
         <is>
-          <t>neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
+          <t>neveen.nashaat@med.asu.edu.eg, marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H111" s="2" t="inlineStr">
@@ -7093,7 +7093,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
+          <t>neveen.nashaat@med.asu.edu.eg, marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
+          <t>neveen.nashaat@med.asu.edu.eg, marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="G177" s="2" t="inlineStr">
         <is>
-          <t>neveen.nashaat@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, marina_atef@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
+          <t>neveen.nashaat@med.asu.edu.eg, marina_atef@med.asu.edu.eg, yassmen.ahmed@med.asu.edu.eg, youstina.magdy@med.asu.edu.eg, 2025/2026</t>
         </is>
       </c>
       <c r="H177" s="2" t="inlineStr">

</xml_diff>